<commit_message>
0.1 prerelease user test
</commit_message>
<xml_diff>
--- a/src/frontend/static/assets/template.xlsx
+++ b/src/frontend/static/assets/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DANIIL\PycharmProjects\crm-backend\src\frontend\static\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DANIIL\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0B7C0A-6BF6-460E-92E3-8BCE4FBFE5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418968C6-9A34-4AA8-8C85-3FB77E057411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="37200" windowHeight="19520" xr2:uid="{68691404-19D1-4706-9885-F95B95F965E0}"/>
+    <workbookView xWindow="1200" yWindow="2080" windowWidth="37200" windowHeight="19520" xr2:uid="{68691404-19D1-4706-9885-F95B95F965E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Текст</t>
   </si>
@@ -52,16 +52,10 @@
     <t>1 - Да</t>
   </si>
   <si>
-    <t>Размер (точно как в ЛК, либо пусто)</t>
-  </si>
-  <si>
     <t>Артикул товара (точно как в ЛК)</t>
   </si>
   <si>
     <t>Внимание! Товары, артикулы и размеры которых будут указаны в этой таблице, должны присутствовать в разделе "Товары" вашей организации в личном кабинете сервиса GreedyBear</t>
-  </si>
-  <si>
-    <t>37-38</t>
   </si>
   <si>
     <t>Отличный товар! Обратите внимание, немного маломерит</t>
@@ -248,24 +242,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -286,9 +274,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -301,18 +286,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -641,110 +620,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F48DDD3-F7AE-4554-BD0D-C18DC4B66F33}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.08984375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.26953125" customWidth="1"/>
-    <col min="12" max="12" width="86.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.08984375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="37.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" customWidth="1"/>
+    <col min="11" max="11" width="86.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" s="12" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="22">
+        <v>11111111111</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="10"/>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="22">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="27">
-        <v>11111111111</v>
-      </c>
-      <c r="B6" s="27" t="s">
+    <row r="7" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="27">
-        <v>1</v>
-      </c>
-      <c r="E6" s="27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="10"/>
+      <c r="E7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>